<commit_message>
Registration Page code and Data update
</commit_message>
<xml_diff>
--- a/BingoData/Bingo_Core_SUITE.xlsx
+++ b/BingoData/Bingo_Core_SUITE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="151">
   <si>
     <t>TestCases</t>
   </si>
@@ -463,6 +463,21 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>80</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,16 +1286,16 @@
       <c r="J10" t="s">
         <v>37</v>
       </c>
-      <c r="K10">
-        <v>3</v>
+      <c r="K10" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L10" t="s">
         <v>38</v>
       </c>
-      <c r="M10">
-        <v>1980</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="M10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>39</v>
       </c>
       <c r="O10" t="s">
@@ -1327,14 +1342,14 @@
       <c r="J11" t="s">
         <v>46</v>
       </c>
-      <c r="K11">
-        <v>3</v>
+      <c r="K11" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L11" t="s">
         <v>38</v>
       </c>
-      <c r="M11">
-        <v>1980</v>
+      <c r="M11" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="N11" t="s">
         <v>86</v>
@@ -1383,14 +1398,14 @@
       <c r="J12" t="s">
         <v>53</v>
       </c>
-      <c r="K12">
-        <v>3</v>
+      <c r="K12" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L12" t="s">
         <v>38</v>
       </c>
-      <c r="M12">
-        <v>1980</v>
+      <c r="M12" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="N12" s="15">
         <v>0.08</v>
@@ -1439,16 +1454,16 @@
       <c r="J13" t="s">
         <v>60</v>
       </c>
-      <c r="K13">
-        <v>3</v>
+      <c r="K13" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L13" t="s">
         <v>38</v>
       </c>
-      <c r="M13">
-        <v>1980</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="M13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>61</v>
       </c>
       <c r="O13" t="s">
@@ -1486,14 +1501,14 @@
       <c r="I14" t="s">
         <v>88</v>
       </c>
-      <c r="K14">
-        <v>3</v>
+      <c r="K14" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L14" t="s">
         <v>38</v>
       </c>
-      <c r="M14">
-        <v>1980</v>
+      <c r="M14" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="O14" t="s">
         <v>89</v>
@@ -1536,14 +1551,14 @@
       <c r="J15" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K15">
-        <v>23</v>
+      <c r="K15" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="L15" t="s">
         <v>95</v>
       </c>
-      <c r="M15">
-        <v>2018</v>
+      <c r="M15" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="N15" s="16">
         <v>80</v>
@@ -1592,14 +1607,14 @@
       <c r="J16" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="K16">
-        <v>3</v>
-      </c>
-      <c r="M16">
-        <v>2015</v>
-      </c>
-      <c r="N16">
-        <v>8</v>
+      <c r="K16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="O16" t="s">
         <v>103</v>
@@ -1631,17 +1646,17 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17">
-        <v>3</v>
+      <c r="K17" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L17" t="s">
         <v>38</v>
       </c>
-      <c r="M17">
-        <v>1980</v>
-      </c>
-      <c r="N17">
-        <v>80</v>
+      <c r="M17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="O17" t="s">
         <v>107</v>
@@ -1681,14 +1696,14 @@
       <c r="I18" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="K18">
-        <v>3</v>
+      <c r="K18" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L18" t="s">
         <v>38</v>
       </c>
-      <c r="M18">
-        <v>2001</v>
+      <c r="M18" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="O18" t="s">
         <v>114</v>
@@ -1734,17 +1749,17 @@
       <c r="J19" t="s">
         <v>67</v>
       </c>
-      <c r="K19">
-        <v>3</v>
+      <c r="K19" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L19" t="s">
         <v>38</v>
       </c>
-      <c r="M19">
-        <v>1980</v>
-      </c>
-      <c r="N19">
-        <v>80</v>
+      <c r="M19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="O19" t="s">
         <v>68</v>
@@ -1788,17 +1803,17 @@
       <c r="J20" t="s">
         <v>67</v>
       </c>
-      <c r="K20">
-        <v>3</v>
+      <c r="K20" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L20" t="s">
         <v>38</v>
       </c>
-      <c r="M20">
-        <v>1980</v>
-      </c>
-      <c r="N20">
-        <v>80</v>
+      <c r="M20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="O20" t="s">
         <v>68</v>
@@ -1844,17 +1859,17 @@
       <c r="J21" t="s">
         <v>67</v>
       </c>
-      <c r="K21">
-        <v>3</v>
+      <c r="K21" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L21" t="s">
         <v>38</v>
       </c>
-      <c r="M21">
-        <v>1980</v>
-      </c>
-      <c r="N21">
-        <v>80</v>
+      <c r="M21" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="O21" t="s">
         <v>68</v>

</xml_diff>